<commit_message>
ready for final rf run on kali
</commit_message>
<xml_diff>
--- a/data/tox_table.xlsx
+++ b/data/tox_table.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Y:\Rscripts\phyto2007\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\bryan\rscripts\esa2017\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -18,6 +18,40 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author>Milstead, William</author>
+  </authors>
+  <commentList>
+    <comment ref="A3" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Milstead, William:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
   <si>
@@ -42,9 +76,6 @@
     <t>saxitoxin</t>
   </si>
   <si>
-    <t>Anabaena</t>
-  </si>
-  <si>
     <t>Anabaenopsis</t>
   </si>
   <si>
@@ -103,13 +134,16 @@
   </si>
   <si>
     <t>Oscillatoria + Phormidium + Planktothrix</t>
+  </si>
+  <si>
+    <t>Anabaena + Dolichospermum</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="19" x14ac:knownFonts="1">
+  <fonts count="24" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -251,6 +285,43 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="16"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="16"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <i/>
+      <sz val="16"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="33">
@@ -594,7 +665,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -602,17 +673,32 @@
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="42">
@@ -968,433 +1054,466 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J13" sqref="J13"/>
+      <selection sqref="A1:H19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="19.140625" style="6" customWidth="1"/>
-    <col min="2" max="2" width="5.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="7.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="6" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="7" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="18.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="9" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="26.42578125" style="4" customWidth="1"/>
+    <col min="2" max="2" width="8.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="26" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.28515625" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="4"/>
-      <c r="B1" s="2" t="s">
+    <row r="1" spans="1:8" s="2" customFormat="1" ht="21" x14ac:dyDescent="0.35">
+      <c r="A1" s="5"/>
+      <c r="B1" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="C1" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="D1" s="7"/>
+      <c r="E1" s="7"/>
+      <c r="F1" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="D1" s="3"/>
-      <c r="E1" s="3"/>
-      <c r="F1" s="3" t="s">
+      <c r="G1" s="7"/>
+      <c r="H1" s="7"/>
+    </row>
+    <row r="2" spans="1:8" s="2" customFormat="1" ht="21" x14ac:dyDescent="0.35">
+      <c r="A2" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="D2" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="E2" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="F2" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="G2" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="H2" s="6" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" ht="42" x14ac:dyDescent="0.35">
+      <c r="A3" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="B3" s="9">
+        <v>643</v>
+      </c>
+      <c r="C3" s="9">
+        <v>312</v>
+      </c>
+      <c r="D3" s="9">
+        <v>3461</v>
+      </c>
+      <c r="E3" s="9">
+        <v>13539</v>
+      </c>
+      <c r="F3" s="9">
+        <v>1</v>
+      </c>
+      <c r="G3" s="9">
+        <v>1</v>
+      </c>
+      <c r="H3" s="9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" ht="21" x14ac:dyDescent="0.35">
+      <c r="A4" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4" s="9">
+        <v>137</v>
+      </c>
+      <c r="C4" s="9">
+        <v>188</v>
+      </c>
+      <c r="D4" s="9">
+        <v>1170</v>
+      </c>
+      <c r="E4" s="9">
+        <v>3536</v>
+      </c>
+      <c r="F4" s="9"/>
+      <c r="G4" s="9">
+        <v>1</v>
+      </c>
+      <c r="H4" s="9"/>
+    </row>
+    <row r="5" spans="1:8" ht="21" x14ac:dyDescent="0.35">
+      <c r="A5" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5" s="9">
+        <v>318</v>
+      </c>
+      <c r="C5" s="9">
+        <v>740</v>
+      </c>
+      <c r="D5" s="9">
+        <v>8527</v>
+      </c>
+      <c r="E5" s="9">
+        <v>25923</v>
+      </c>
+      <c r="F5" s="9">
+        <v>1</v>
+      </c>
+      <c r="G5" s="9"/>
+      <c r="H5" s="9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" ht="21" x14ac:dyDescent="0.35">
+      <c r="A6" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6" s="9">
+        <v>397</v>
+      </c>
+      <c r="C6" s="9">
+        <v>110</v>
+      </c>
+      <c r="D6" s="9">
+        <v>13406</v>
+      </c>
+      <c r="E6" s="9">
+        <v>158052</v>
+      </c>
+      <c r="F6" s="9"/>
+      <c r="G6" s="9">
+        <v>1</v>
+      </c>
+      <c r="H6" s="9"/>
+    </row>
+    <row r="7" spans="1:8" ht="21" x14ac:dyDescent="0.35">
+      <c r="A7" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="B7" s="9">
+        <v>166</v>
+      </c>
+      <c r="C7" s="9">
+        <v>891</v>
+      </c>
+      <c r="D7" s="9">
+        <v>6094</v>
+      </c>
+      <c r="E7" s="9">
+        <v>36273</v>
+      </c>
+      <c r="F7" s="9"/>
+      <c r="G7" s="9">
+        <v>1</v>
+      </c>
+      <c r="H7" s="9"/>
+    </row>
+    <row r="8" spans="1:8" ht="21" x14ac:dyDescent="0.35">
+      <c r="A8" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="B8" s="9">
+        <v>47</v>
+      </c>
+      <c r="C8" s="9">
+        <v>438</v>
+      </c>
+      <c r="D8" s="9">
+        <v>2481</v>
+      </c>
+      <c r="E8" s="9">
+        <v>5268</v>
+      </c>
+      <c r="F8" s="9">
+        <v>1</v>
+      </c>
+      <c r="G8" s="9"/>
+      <c r="H8" s="9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" ht="21" x14ac:dyDescent="0.35">
+      <c r="A9" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="B9" s="9">
+        <v>143</v>
+      </c>
+      <c r="C9" s="9">
+        <v>1062</v>
+      </c>
+      <c r="D9" s="9">
+        <v>3271</v>
+      </c>
+      <c r="E9" s="9">
+        <v>8121</v>
+      </c>
+      <c r="F9" s="9"/>
+      <c r="G9" s="9">
+        <v>1</v>
+      </c>
+      <c r="H9" s="9"/>
+    </row>
+    <row r="10" spans="1:8" ht="21" x14ac:dyDescent="0.35">
+      <c r="A10" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="B10" s="9">
+        <v>80</v>
+      </c>
+      <c r="C10" s="9">
+        <v>676</v>
+      </c>
+      <c r="D10" s="9">
+        <v>13383</v>
+      </c>
+      <c r="E10" s="9">
+        <v>51263</v>
+      </c>
+      <c r="F10" s="9"/>
+      <c r="G10" s="9">
+        <v>1</v>
+      </c>
+      <c r="H10" s="9"/>
+    </row>
+    <row r="11" spans="1:8" ht="21" x14ac:dyDescent="0.35">
+      <c r="A11" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="B11" s="9">
+        <v>268</v>
+      </c>
+      <c r="C11" s="9">
+        <v>174</v>
+      </c>
+      <c r="D11" s="9">
+        <v>1853</v>
+      </c>
+      <c r="E11" s="9">
+        <v>5620</v>
+      </c>
+      <c r="F11" s="9">
+        <v>1</v>
+      </c>
+      <c r="G11" s="9">
+        <v>1</v>
+      </c>
+      <c r="H11" s="9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" ht="21" x14ac:dyDescent="0.35">
+      <c r="A12" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="B12" s="9">
+        <v>661</v>
+      </c>
+      <c r="C12" s="9">
+        <v>2953</v>
+      </c>
+      <c r="D12" s="9">
+        <v>27974</v>
+      </c>
+      <c r="E12" s="9">
+        <v>204147</v>
+      </c>
+      <c r="F12" s="9"/>
+      <c r="G12" s="9">
+        <v>1</v>
+      </c>
+      <c r="H12" s="9"/>
+    </row>
+    <row r="13" spans="1:8" ht="63" x14ac:dyDescent="0.35">
+      <c r="A13" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="G1" s="3"/>
-      <c r="H1" s="3"/>
-    </row>
-    <row r="2" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="F2" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="G2" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="H2" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="B3">
-        <v>643</v>
-      </c>
-      <c r="C3">
-        <v>312</v>
-      </c>
-      <c r="D3">
-        <v>3461</v>
-      </c>
-      <c r="E3">
-        <v>13539</v>
-      </c>
-      <c r="F3" s="1">
-        <v>1</v>
-      </c>
-      <c r="G3" s="1">
-        <v>1</v>
-      </c>
-      <c r="H3" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="B4">
-        <v>137</v>
-      </c>
-      <c r="C4">
-        <v>188</v>
-      </c>
-      <c r="D4">
-        <v>1170</v>
-      </c>
-      <c r="E4">
-        <v>3536</v>
-      </c>
-      <c r="G4" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="B5">
-        <v>318</v>
-      </c>
-      <c r="C5">
-        <v>740</v>
-      </c>
-      <c r="D5">
-        <v>8527</v>
-      </c>
-      <c r="E5">
-        <v>25923</v>
-      </c>
-      <c r="F5" s="1">
-        <v>1</v>
-      </c>
-      <c r="H5" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="B6">
-        <v>397</v>
-      </c>
-      <c r="C6">
-        <v>110</v>
-      </c>
-      <c r="D6">
-        <v>13406</v>
-      </c>
-      <c r="E6">
-        <v>158052</v>
-      </c>
-      <c r="G6" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A7" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="B7">
-        <v>166</v>
-      </c>
-      <c r="C7">
-        <v>891</v>
-      </c>
-      <c r="D7">
-        <v>6094</v>
-      </c>
-      <c r="E7">
-        <v>36273</v>
-      </c>
-      <c r="G7" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A8" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="B8">
-        <v>47</v>
-      </c>
-      <c r="C8">
-        <v>438</v>
-      </c>
-      <c r="D8">
-        <v>2481</v>
-      </c>
-      <c r="E8">
-        <v>5268</v>
-      </c>
-      <c r="F8" s="1">
-        <v>1</v>
-      </c>
-      <c r="H8" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A9" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="B9">
-        <v>143</v>
-      </c>
-      <c r="C9">
-        <v>1062</v>
-      </c>
-      <c r="D9">
-        <v>3271</v>
-      </c>
-      <c r="E9">
-        <v>8121</v>
-      </c>
-      <c r="G9" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A10" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="B10">
-        <v>80</v>
-      </c>
-      <c r="C10">
-        <v>676</v>
-      </c>
-      <c r="D10">
-        <v>13383</v>
-      </c>
-      <c r="E10">
-        <v>51263</v>
-      </c>
-      <c r="G10" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A11" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="B11">
-        <v>268</v>
-      </c>
-      <c r="C11">
-        <v>174</v>
-      </c>
-      <c r="D11">
-        <v>1853</v>
-      </c>
-      <c r="E11">
-        <v>5620</v>
-      </c>
-      <c r="F11" s="1">
-        <v>1</v>
-      </c>
-      <c r="G11" s="1">
-        <v>1</v>
-      </c>
-      <c r="H11" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A12" s="5" t="s">
+      <c r="B13" s="9">
+        <v>521</v>
+      </c>
+      <c r="C13" s="9">
+        <v>239</v>
+      </c>
+      <c r="D13" s="9">
+        <v>2929</v>
+      </c>
+      <c r="E13" s="9">
+        <v>14601</v>
+      </c>
+      <c r="F13" s="9"/>
+      <c r="G13" s="9">
+        <v>1</v>
+      </c>
+      <c r="H13" s="9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" ht="21" x14ac:dyDescent="0.35">
+      <c r="A14" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="B12">
-        <v>661</v>
-      </c>
-      <c r="C12">
-        <v>2953</v>
-      </c>
-      <c r="D12">
-        <v>27974</v>
-      </c>
-      <c r="E12">
-        <v>204147</v>
-      </c>
-      <c r="G12" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" ht="45" x14ac:dyDescent="0.25">
-      <c r="A13" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="B13">
-        <v>521</v>
-      </c>
-      <c r="C13">
-        <v>239</v>
-      </c>
-      <c r="D13">
-        <v>2929</v>
-      </c>
-      <c r="E13">
-        <v>14601</v>
-      </c>
-      <c r="G13" s="1">
-        <v>1</v>
-      </c>
-      <c r="H13" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A14" s="5" t="s">
+      <c r="B14" s="9">
+        <v>93</v>
+      </c>
+      <c r="C14" s="9">
+        <v>305</v>
+      </c>
+      <c r="D14" s="9">
+        <v>1714</v>
+      </c>
+      <c r="E14" s="9">
+        <v>5530</v>
+      </c>
+      <c r="F14" s="9"/>
+      <c r="G14" s="9">
+        <v>1</v>
+      </c>
+      <c r="H14" s="9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" ht="21" x14ac:dyDescent="0.35">
+      <c r="A15" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="B14">
-        <v>93</v>
-      </c>
-      <c r="C14">
-        <v>305</v>
-      </c>
-      <c r="D14">
-        <v>1714</v>
-      </c>
-      <c r="E14">
-        <v>5530</v>
-      </c>
-      <c r="G14" s="1">
-        <v>1</v>
-      </c>
-      <c r="H14" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A15" s="5" t="s">
+      <c r="B15" s="9">
+        <v>106</v>
+      </c>
+      <c r="C15" s="9">
+        <v>323</v>
+      </c>
+      <c r="D15" s="9">
+        <v>1802</v>
+      </c>
+      <c r="E15" s="9">
+        <v>6861</v>
+      </c>
+      <c r="F15" s="9"/>
+      <c r="G15" s="9">
+        <v>1</v>
+      </c>
+      <c r="H15" s="9"/>
+    </row>
+    <row r="16" spans="1:8" ht="21" x14ac:dyDescent="0.35">
+      <c r="A16" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="B15">
-        <v>106</v>
-      </c>
-      <c r="C15">
-        <v>323</v>
-      </c>
-      <c r="D15">
-        <v>1802</v>
-      </c>
-      <c r="E15">
-        <v>6861</v>
-      </c>
-      <c r="G15" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A16" s="5" t="s">
+      <c r="B16" s="9">
+        <v>134</v>
+      </c>
+      <c r="C16" s="9">
+        <v>74</v>
+      </c>
+      <c r="D16" s="9">
+        <v>1328</v>
+      </c>
+      <c r="E16" s="9">
+        <v>7030</v>
+      </c>
+      <c r="F16" s="9">
+        <v>1</v>
+      </c>
+      <c r="G16" s="9"/>
+      <c r="H16" s="9"/>
+    </row>
+    <row r="17" spans="1:8" ht="21" x14ac:dyDescent="0.35">
+      <c r="A17" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="B16">
-        <v>134</v>
-      </c>
-      <c r="C16">
-        <v>74</v>
-      </c>
-      <c r="D16">
-        <v>1328</v>
-      </c>
-      <c r="E16">
-        <v>7030</v>
-      </c>
-      <c r="F16" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A17" s="5" t="s">
+      <c r="B17" s="9">
+        <v>26</v>
+      </c>
+      <c r="C17" s="9">
+        <v>703</v>
+      </c>
+      <c r="D17" s="9">
+        <v>2030</v>
+      </c>
+      <c r="E17" s="9">
+        <v>5357</v>
+      </c>
+      <c r="F17" s="9"/>
+      <c r="G17" s="9">
+        <v>1</v>
+      </c>
+      <c r="H17" s="9"/>
+    </row>
+    <row r="18" spans="1:8" ht="21" x14ac:dyDescent="0.35">
+      <c r="A18" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="B17">
-        <v>26</v>
-      </c>
-      <c r="C17">
-        <v>703</v>
-      </c>
-      <c r="D17">
-        <v>2030</v>
-      </c>
-      <c r="E17">
-        <v>5357</v>
-      </c>
-      <c r="G17" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A18" s="5" t="s">
+      <c r="B18" s="9">
+        <v>283</v>
+      </c>
+      <c r="C18" s="9">
+        <v>201</v>
+      </c>
+      <c r="D18" s="9">
+        <v>407</v>
+      </c>
+      <c r="E18" s="9">
+        <v>591</v>
+      </c>
+      <c r="F18" s="9"/>
+      <c r="G18" s="9">
+        <v>1</v>
+      </c>
+      <c r="H18" s="9"/>
+    </row>
+    <row r="19" spans="1:8" ht="21" x14ac:dyDescent="0.35">
+      <c r="A19" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="B18">
-        <v>283</v>
-      </c>
-      <c r="C18">
-        <v>201</v>
-      </c>
-      <c r="D18">
-        <v>407</v>
-      </c>
-      <c r="E18">
-        <v>591</v>
-      </c>
-      <c r="G18" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A19" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="B19">
+      <c r="B19" s="9">
         <v>187</v>
       </c>
-      <c r="C19">
+      <c r="C19" s="9">
         <v>490</v>
       </c>
-      <c r="D19">
+      <c r="D19" s="9">
         <v>2421</v>
       </c>
-      <c r="E19">
+      <c r="E19" s="9">
         <v>8951</v>
       </c>
-      <c r="G19" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A20" s="5"/>
+      <c r="F19" s="9"/>
+      <c r="G19" s="9">
+        <v>1</v>
+      </c>
+      <c r="H19" s="9"/>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A20" s="3"/>
+      <c r="B20" s="10"/>
+      <c r="C20" s="10"/>
+      <c r="D20" s="10"/>
+      <c r="E20" s="10"/>
+      <c r="F20" s="11"/>
+      <c r="G20" s="11"/>
+      <c r="H20" s="11"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -1403,5 +1522,6 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>